<commit_message>
feat: add xlsx sample for group upload
</commit_message>
<xml_diff>
--- a/xlsx/group_test.xlsx
+++ b/xlsx/group_test.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\xuwenjie\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project\CloneProject\GoProject\casdoor\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D97642E6-FF1D-4EF0-A487-46B1D4F871FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44D59FA0-F9DE-4FED-8289-5F436421397D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{3EB5954F-C938-4443-BD63-7F75894AB0CB}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="32">
   <si>
     <t>owner</t>
   </si>
@@ -50,9 +50,6 @@
     <t>type</t>
   </si>
   <si>
-    <t>users</t>
-  </si>
-  <si>
     <t>title</t>
   </si>
   <si>
@@ -74,25 +71,12 @@
     <t>contact_email</t>
   </si>
   <si>
-    <t>parent_name</t>
-  </si>
-  <si>
     <t>is_top_group</t>
   </si>
   <si>
-    <t>have_children</t>
-  </si>
-  <si>
     <t>is_enabled</t>
   </si>
   <si>
-    <t>虚拟组</t>
-  </si>
-  <si>
-    <t>虚拟组</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>built-in</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -101,73 +85,67 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>team1</t>
-  </si>
-  <si>
     <t>2022-03-21T10:00:00+08:00</t>
   </si>
   <si>
-    <t>Team One</t>
-  </si>
-  <si>
-    <t>JohnDoe</t>
-  </si>
-  <si>
-    <t>team1@example.com</t>
-  </si>
-  <si>
-    <t>team2</t>
-  </si>
-  <si>
     <t>2022-03-22T11:00:00+08:00</t>
   </si>
   <si>
-    <t>Team Two</t>
-  </si>
-  <si>
-    <t>JaneDoe</t>
-  </si>
-  <si>
-    <t>team2@example.com</t>
-  </si>
-  <si>
-    <t>team3</t>
-  </si>
-  <si>
     <t>2022-03-25T14:00:00+08:00</t>
   </si>
   <si>
-    <t>Team Three</t>
-  </si>
-  <si>
-    <t>JoeSmith</t>
-  </si>
-  <si>
-    <t>team3@example.com</t>
-  </si>
-  <si>
-    <t>subteam1</t>
-  </si>
-  <si>
     <t>2022-03-26T15:00:00+08:00</t>
   </si>
   <si>
-    <t>Subteam One</t>
-  </si>
-  <si>
-    <t>subteam1@example.com</t>
-  </si>
-  <si>
-    <t>subteam2</t>
-  </si>
-  <si>
     <t>2022-03-27T16:00:00+08:00</t>
   </si>
   <si>
-    <t>Subteam Two</t>
-  </si>
-  <si>
-    <t>subteam2@example.com</t>
+    <t>Virtual</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>group_sddfmb</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>group_doango</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>group_popdae</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>group_ffadef</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>group_dassae</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>New Group - sddfmb</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>New Group - doango</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>New Group - popdae</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>New Group - dassae</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>New Group - ffadef</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>null</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -558,15 +536,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4652F0FB-4026-4564-BC02-18A94AFDE440}">
-  <dimension ref="A1:Q6"/>
+  <dimension ref="A1:N6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N9" sqref="N9"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -574,239 +552,200 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" t="s">
         <v>8</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>9</v>
-      </c>
-      <c r="E1" t="s">
-        <v>10</v>
       </c>
       <c r="F1" t="s">
         <v>2</v>
       </c>
       <c r="G1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H1" t="s">
         <v>3</v>
       </c>
       <c r="I1" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="J1" t="s">
+        <v>11</v>
+      </c>
+      <c r="K1" t="s">
+        <v>4</v>
+      </c>
+      <c r="L1" t="s">
+        <v>5</v>
+      </c>
+      <c r="M1" t="s">
+        <v>6</v>
+      </c>
+      <c r="N1" t="s">
         <v>12</v>
       </c>
-      <c r="K1" t="s">
-        <v>13</v>
-      </c>
-      <c r="L1" t="s">
-        <v>4</v>
-      </c>
-      <c r="M1" t="s">
-        <v>5</v>
-      </c>
-      <c r="N1" t="s">
-        <v>6</v>
-      </c>
-      <c r="O1" t="s">
-        <v>14</v>
-      </c>
-      <c r="P1" t="s">
-        <v>7</v>
-      </c>
-      <c r="Q1" t="s">
+    </row>
+    <row r="2" spans="1:14" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2" t="s">
         <v>15</v>
       </c>
+      <c r="D2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2" t="s">
+        <v>26</v>
+      </c>
+      <c r="H2" t="s">
+        <v>20</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="J2">
+        <v>1</v>
+      </c>
+      <c r="M2" t="s">
+        <v>31</v>
+      </c>
+      <c r="N2">
+        <v>1</v>
+      </c>
     </row>
-    <row r="2" spans="1:17" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D2" t="s">
-        <v>21</v>
-      </c>
-      <c r="E2" t="s">
+    <row r="3" spans="1:14" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" t="s">
         <v>22</v>
       </c>
-      <c r="F2" t="s">
-        <v>23</v>
-      </c>
-      <c r="G2" t="s">
-        <v>24</v>
-      </c>
-      <c r="H2" t="s">
-        <v>17</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="K2">
-        <v>0</v>
-      </c>
-      <c r="Q2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:17" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B3" t="s">
-        <v>25</v>
-      </c>
       <c r="C3" t="s">
-        <v>26</v>
+        <v>16</v>
       </c>
       <c r="D3" t="s">
-        <v>26</v>
+        <v>16</v>
       </c>
       <c r="E3" t="s">
         <v>27</v>
       </c>
-      <c r="F3" t="s">
+      <c r="H3" t="s">
+        <v>20</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="J3">
+        <v>1</v>
+      </c>
+      <c r="M3" t="s">
+        <v>31</v>
+      </c>
+      <c r="N3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E4" t="s">
         <v>28</v>
       </c>
-      <c r="G3" t="s">
+      <c r="H4" t="s">
+        <v>20</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="J4">
+        <v>1</v>
+      </c>
+      <c r="M4" t="s">
+        <v>31</v>
+      </c>
+      <c r="N4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5" t="s">
+        <v>18</v>
+      </c>
+      <c r="E5" t="s">
+        <v>30</v>
+      </c>
+      <c r="H5" t="s">
+        <v>20</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="J5">
+        <v>1</v>
+      </c>
+      <c r="M5" t="s">
+        <v>31</v>
+      </c>
+      <c r="N5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" t="s">
+        <v>25</v>
+      </c>
+      <c r="C6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D6" t="s">
+        <v>19</v>
+      </c>
+      <c r="E6" t="s">
         <v>29</v>
       </c>
-      <c r="H3" t="s">
-        <v>16</v>
-      </c>
-      <c r="I3" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="J3" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="K3">
-        <v>0</v>
-      </c>
-      <c r="Q3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:17" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B4" t="s">
-        <v>30</v>
-      </c>
-      <c r="C4" t="s">
+      <c r="H6" t="s">
+        <v>20</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="J6">
+        <v>1</v>
+      </c>
+      <c r="M6" t="s">
         <v>31</v>
       </c>
-      <c r="D4" t="s">
-        <v>31</v>
-      </c>
-      <c r="E4" t="s">
-        <v>32</v>
-      </c>
-      <c r="F4" t="s">
-        <v>33</v>
-      </c>
-      <c r="G4" t="s">
-        <v>34</v>
-      </c>
-      <c r="H4" t="s">
-        <v>17</v>
-      </c>
-      <c r="I4" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="J4" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="K4">
-        <v>0</v>
-      </c>
-      <c r="Q4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:17" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A5" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B5" t="s">
-        <v>35</v>
-      </c>
-      <c r="C5" t="s">
-        <v>36</v>
-      </c>
-      <c r="D5" t="s">
-        <v>36</v>
-      </c>
-      <c r="E5" t="s">
-        <v>37</v>
-      </c>
-      <c r="F5" t="s">
-        <v>28</v>
-      </c>
-      <c r="G5" t="s">
-        <v>38</v>
-      </c>
-      <c r="H5" t="s">
-        <v>16</v>
-      </c>
-      <c r="I5" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="J5" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="K5">
-        <v>0</v>
-      </c>
-      <c r="Q5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:17" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A6" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B6" t="s">
-        <v>39</v>
-      </c>
-      <c r="C6" t="s">
-        <v>40</v>
-      </c>
-      <c r="D6" t="s">
-        <v>40</v>
-      </c>
-      <c r="E6" t="s">
-        <v>41</v>
-      </c>
-      <c r="F6" t="s">
-        <v>23</v>
-      </c>
-      <c r="G6" t="s">
-        <v>42</v>
-      </c>
-      <c r="H6" t="s">
-        <v>17</v>
-      </c>
-      <c r="I6" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="J6" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="K6">
-        <v>0</v>
-      </c>
-      <c r="Q6">
-        <v>0</v>
+      <c r="N6">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>